<commit_message>
Added option to use List for TransactionData
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin.Zhou\Documents\UiPath\REFConverter\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{567B79B9-5536-4AA3-A076-0104D2AE9EAC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D5ECBEC-35AD-4405-A0D2-97A0FCF52CA4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6552" yWindow="2508" windowWidth="23040" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1908" yWindow="3468" windowWidth="27660" windowHeight="11592" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="106">
   <si>
     <t>Name</t>
   </si>
@@ -316,6 +316,30 @@
   </si>
   <si>
     <t>Assembly for Match variable type</t>
+  </si>
+  <si>
+    <t>List</t>
+  </si>
+  <si>
+    <t>ListNamespace</t>
+  </si>
+  <si>
+    <t>ListAssembly</t>
+  </si>
+  <si>
+    <t>scg:List(&lt;T&gt;)</t>
+  </si>
+  <si>
+    <t>System.Collections.Generic</t>
+  </si>
+  <si>
+    <t>List variable type with namespace</t>
+  </si>
+  <si>
+    <t>Namespace for List variable type</t>
+  </si>
+  <si>
+    <t>Assembly for List variable type</t>
   </si>
 </sst>
 </file>
@@ -689,7 +713,7 @@
   <dimension ref="A1:Z1012"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1055,22 +1079,52 @@
         <v>97</v>
       </c>
     </row>
-    <row r="33" ht="14.25" customHeight="1"/>
-    <row r="34" ht="14.25" customHeight="1"/>
-    <row r="35" ht="14.25" customHeight="1"/>
-    <row r="36" ht="14.25" customHeight="1"/>
-    <row r="37" ht="14.25" customHeight="1"/>
-    <row r="38" ht="14.25" customHeight="1"/>
-    <row r="39" ht="14.25" customHeight="1"/>
-    <row r="40" ht="14.25" customHeight="1"/>
-    <row r="41" ht="14.25" customHeight="1"/>
-    <row r="42" ht="14.25" customHeight="1"/>
-    <row r="43" ht="14.25" customHeight="1"/>
-    <row r="44" ht="14.25" customHeight="1"/>
-    <row r="45" ht="14.25" customHeight="1"/>
-    <row r="46" ht="14.25" customHeight="1"/>
-    <row r="47" ht="14.25" customHeight="1"/>
-    <row r="48" ht="14.25" customHeight="1"/>
+    <row r="33" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A33" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B33" t="s">
+        <v>101</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A34" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B34" t="s">
+        <v>102</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A35" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B35" t="s">
+        <v>102</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="37" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="38" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="39" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="40" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="41" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="42" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="43" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="44" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="45" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="46" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="47" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="48" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="49" ht="14.25" customHeight="1"/>
     <row r="50" ht="14.25" customHeight="1"/>
     <row r="51" ht="14.25" customHeight="1"/>

</xml_diff>